<commit_message>
Ajout MakerFaire et MAJ dsPIC 7robinch
</commit_message>
<xml_diff>
--- a/CalculTimers.xlsx
+++ b/CalculTimers.xlsx
@@ -83,7 +83,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="2">
     <dxf>
       <font>
         <condense val="0"/>
@@ -105,54 +105,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -540,7 +492,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -567,19 +519,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>4.9999999999999998E-7</v>
+        <v>0.1</v>
       </c>
       <c r="D5">
         <f>B5</f>
-        <v>4.9999999999999998E-7</v>
+        <v>0.1</v>
       </c>
       <c r="E5">
         <f>1/B5</f>
-        <v>2000000</v>
-      </c>
-      <c r="F5" s="1">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2">
         <f>(B1/B2)*B5</f>
-        <v>20</v>
+        <v>15625</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -587,19 +539,19 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>400</v>
+        <v>50</v>
       </c>
       <c r="D6">
         <f>1/B6</f>
-        <v>2.5000000000000001E-3</v>
+        <v>0.02</v>
       </c>
       <c r="E6">
         <f>B6</f>
-        <v>400</v>
+        <v>50</v>
       </c>
       <c r="F6" s="2">
         <f>(B1/B2)/B6</f>
-        <v>100000</v>
+        <v>3125</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -607,19 +559,19 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>500</v>
+        <v>3125</v>
       </c>
       <c r="D7" s="1">
         <f>B7/(B1/B2)</f>
-        <v>1.2500000000000001E-5</v>
+        <v>0.02</v>
       </c>
       <c r="E7" s="2">
         <f>(B1/B2)/B7</f>
-        <v>80000</v>
+        <v>50</v>
       </c>
       <c r="F7">
         <f>B7</f>
-        <v>500</v>
+        <v>3125</v>
       </c>
     </row>
   </sheetData>
@@ -632,6 +584,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>